<commit_message>
Submit accreditamento scheda vaccinazione e Certificato Vaccinale
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DXCTECHNOLO/dxc/sinfonia-vaccini/2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111DXCTECHNOLO/dxc/sinfonia-vaccini/2.0/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dxcportal.sharepoint.com/sites/PiattaformaVaccinaleSinfonia/Shared Documents/Piattaforma Vaccinale 2.0/Analysis And Design/Integrazione-fse/accreditamento/GATEWAY/A1#111DXCTECHNOLO/dxc/sinfonia-vaccini/2.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asaginario\Documents\Lavoro\Progetti\SGISanita-Projects\FSE-TestCaseAccreditamento\GATEWAY\A1#111DXCTECHNOLO\dxc\sinfonia-vaccini\2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{E2409B4A-9EBD-4507-A035-294389A3178D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03839A53-89A2-4292-AAA9-E0C3C50C0898}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB5D104-DA9D-426C-89AC-F3041DDE2D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$51</definedName>
     <definedName name="filtro" localSheetId="2">TestCases!$A$9:$S$10</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="233">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -734,6 +734,268 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150.4.4.204.859f21dd3c5c72a507efab6bd3cdb8c396219efeddd908bae22a9dc478620663.06c10b9c2c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_TOKEN_JWT_CERT_VAC_KO</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_TOKEN_JWT_CAMPO_CERT_VAC_KO</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CERT_VAC_TIMEOUT</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT5_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-05-11T15:07:32Z</t>
+  </si>
+  <si>
+    <t>54a982bf1fe81952</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.75877f466c4515833b756f7f42b551491927b78b2775850632f26c9ce055839e.cb80e999cb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT6_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT7_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>57da7c7ad6b0680e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.75877f466c4515833b756f7f42b551491927b78b2775850632f26c9ce055839e.dfe56f9f4c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT8_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>30fca32877bea49e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.75877f466c4515833b756f7f42b551491927b78b2775850632f26c9ce055839e.a8b1b53d00^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT9_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>146230514424304e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.75877f466c4515833b756f7f42b551491927b78b2775850632f26c9ce055839e.5beef294eb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT10_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>fbb812ebaff4b92a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.75877f466c4515833b756f7f42b551491927b78b2775850632f26c9ce055839e.006d7c9efd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT11_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>64e4a0363d9c35de</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.75877f466c4515833b756f7f42b551491927b78b2775850632f26c9ce055839e.09219123ec^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT12_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>549fd604d5b46b0d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.75877f466c4515833b756f7f42b551491927b78b2775850632f26c9ce055839e.10f9061138^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT13_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>32eab144d633894f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.75877f466c4515833b756f7f42b551491927b78b2775850632f26c9ce055839e.dc7a277fd5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT14_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>f5bba4fb747c1948</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.75877f466c4515833b756f7f42b551491927b78b2775850632f26c9ce055839e.40e56e3a98^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT15_KO</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>5d4760bcb069c5d8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.75877f466c4515833b756f7f42b551491927b78b2775850632f26c9ce055839e.998ddbc736^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT16_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>b74da2ec830cbb1a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.75877f466c4515833b756f7f42b551491927b78b2775850632f26c9ce055839e.d5740ad0aa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_CERT_VAC_CT17_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-05-10T15:29:20Z</t>
+  </si>
+  <si>
+    <t>0fb5479234f1c0bf</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.75877f466c4515833b756f7f42b551491927b78b2775850632f26c9ce055839e.84c1e16cee^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-12T10:41:20Z</t>
+  </si>
+  <si>
+    <t>65354110eee60ae0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.0caa65f702128f218163d49362d1e8faafd3ee1502e7cfbf3c5ff04731a06f50.9c69c3c3a1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-12T11:41:20Z</t>
+  </si>
+  <si>
+    <t>366754ad0c6013b5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.8c21ca1b2e018ded516266256778abe98e9e25498ac781019ad87b7f3b325132.dcfd4184cb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-12T15:29:20Z</t>
+  </si>
+  <si>
+    <t>5d7d34789516de8a</t>
+  </si>
+  <si>
+    <t>e466c2b5492906fc</t>
+  </si>
+  <si>
+    <t>2023-05-12T13:41:20Z</t>
+  </si>
+  <si>
+    <t>118eca65cdd9a86a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.50b3dc5d32cc3e16e4330e4a4d36eeabcdea780d84aaed797129d80d5785674c.df1e9621b7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>418d4d71fd12ba03</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.8c21ca1b2e018ded516266256778abe98e9e25498ac781019ad87b7f3b325132.31a3a04055^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1204,6 +1466,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1225,6 +1488,40 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3682,11 +3979,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T649"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="F46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomRight" activeCell="L55" sqref="L55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3725,12 +4022,12 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="50"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3748,14 +4045,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="57" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="50"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -3773,12 +4070,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="57" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="D4" s="49"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -3797,12 +4094,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="57" t="s">
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="50"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -3820,8 +4117,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="46"/>
-      <c r="B6" s="47"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4149,9 +4446,13 @@
       <c r="L14" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="M14" s="25"/>
+      <c r="M14" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
+      <c r="O14" s="25" t="s">
+        <v>62</v>
+      </c>
       <c r="P14" s="25" t="s">
         <v>106</v>
       </c>
@@ -4197,9 +4498,13 @@
       <c r="L15" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="M15" s="25"/>
+      <c r="M15" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
+      <c r="O15" s="25" t="s">
+        <v>62</v>
+      </c>
       <c r="P15" s="25" t="s">
         <v>106</v>
       </c>
@@ -4282,8 +4587,12 @@
         <v>62</v>
       </c>
       <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
+      <c r="L17" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M17" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="N17" s="25"/>
       <c r="O17" s="25" t="s">
         <v>152</v>
@@ -4368,8 +4677,12 @@
         <v>62</v>
       </c>
       <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
+      <c r="L19" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M19" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="N19" s="25"/>
       <c r="O19" s="25" t="s">
         <v>152</v>
@@ -4419,7 +4732,9 @@
       <c r="L20" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="M20" s="25"/>
+      <c r="M20" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="N20" s="25"/>
       <c r="O20" s="25" t="s">
         <v>62</v>
@@ -4466,8 +4781,12 @@
         <v>62</v>
       </c>
       <c r="K21" s="24"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
+      <c r="L21" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M21" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="N21" s="25"/>
       <c r="O21" s="25" t="s">
         <v>152</v>
@@ -4514,8 +4833,12 @@
         <v>152</v>
       </c>
       <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
+      <c r="L22" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M22" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="N22" s="25"/>
       <c r="O22" s="25" t="s">
         <v>152</v>
@@ -4562,8 +4885,12 @@
         <v>152</v>
       </c>
       <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
+      <c r="L23" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M23" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="N23" s="25"/>
       <c r="O23" s="25" t="s">
         <v>62</v>
@@ -4610,8 +4937,12 @@
         <v>62</v>
       </c>
       <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
+      <c r="L24" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M24" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="N24" s="25"/>
       <c r="O24" s="25" t="s">
         <v>62</v>
@@ -4658,8 +4989,12 @@
         <v>62</v>
       </c>
       <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
+      <c r="L25" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M25" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="N25" s="25"/>
       <c r="O25" s="25" t="s">
         <v>62</v>
@@ -4706,8 +5041,12 @@
         <v>62</v>
       </c>
       <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
+      <c r="L26" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M26" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="N26" s="25"/>
       <c r="O26" s="25" t="s">
         <v>62</v>
@@ -4754,8 +5093,12 @@
         <v>62</v>
       </c>
       <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
+      <c r="L27" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M27" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="N27" s="25"/>
       <c r="O27" s="25" t="s">
         <v>62</v>
@@ -4802,8 +5145,12 @@
         <v>62</v>
       </c>
       <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
+      <c r="L28" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M28" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="N28" s="25"/>
       <c r="O28" s="25" t="s">
         <v>62</v>
@@ -4850,8 +5197,12 @@
         <v>62</v>
       </c>
       <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
+      <c r="L29" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M29" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="N29" s="25"/>
       <c r="O29" s="25" t="s">
         <v>62</v>
@@ -4898,8 +5249,12 @@
         <v>62</v>
       </c>
       <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
+      <c r="L30" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M30" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="N30" s="25"/>
       <c r="O30" s="25" t="s">
         <v>62</v>
@@ -4914,7 +5269,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="120">
+    <row r="31" spans="1:20" ht="120.75" thickBot="1">
       <c r="A31" s="20">
         <v>121</v>
       </c>
@@ -4946,8 +5301,12 @@
         <v>62</v>
       </c>
       <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
+      <c r="L31" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M31" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="N31" s="25"/>
       <c r="O31" s="25" t="s">
         <v>62</v>
@@ -4962,347 +5321,989 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="15"/>
-    </row>
-    <row r="33" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
-      <c r="Q33" s="13"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="15"/>
-    </row>
-    <row r="34" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="13"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="15"/>
-    </row>
-    <row r="35" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="15"/>
-    </row>
-    <row r="36" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-      <c r="Q36" s="13"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="15"/>
-    </row>
-    <row r="37" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
-      <c r="P37" s="13"/>
-      <c r="Q37" s="13"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="15"/>
-    </row>
-    <row r="38" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="13"/>
-      <c r="O38" s="13"/>
-      <c r="P38" s="13"/>
-      <c r="Q38" s="13"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="15"/>
-    </row>
-    <row r="39" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="13"/>
-      <c r="K39" s="13"/>
-      <c r="L39" s="13"/>
-      <c r="M39" s="13"/>
-      <c r="N39" s="13"/>
-      <c r="O39" s="13"/>
-      <c r="P39" s="13"/>
-      <c r="Q39" s="13"/>
-      <c r="R39" s="14"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="15"/>
-    </row>
-    <row r="40" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="13"/>
-      <c r="P40" s="13"/>
-      <c r="Q40" s="13"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="15"/>
-    </row>
-    <row r="41" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="13"/>
-      <c r="P41" s="13"/>
-      <c r="Q41" s="13"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="2"/>
-      <c r="T41" s="15"/>
-    </row>
-    <row r="42" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="13"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="13"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="2"/>
-      <c r="T42" s="15"/>
-    </row>
-    <row r="43" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="13"/>
-      <c r="K43" s="13"/>
-      <c r="L43" s="13"/>
-      <c r="M43" s="13"/>
-      <c r="N43" s="13"/>
-      <c r="O43" s="13"/>
-      <c r="P43" s="13"/>
-      <c r="Q43" s="13"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="2"/>
-      <c r="T43" s="15"/>
-    </row>
-    <row r="44" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
-      <c r="M44" s="13"/>
-      <c r="N44" s="13"/>
-      <c r="O44" s="13"/>
-      <c r="P44" s="13"/>
-      <c r="Q44" s="13"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="15"/>
-    </row>
-    <row r="45" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="13"/>
-      <c r="K45" s="13"/>
-      <c r="L45" s="13"/>
-      <c r="M45" s="13"/>
-      <c r="N45" s="13"/>
-      <c r="O45" s="13"/>
-      <c r="P45" s="13"/>
-      <c r="Q45" s="13"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="15"/>
-    </row>
-    <row r="46" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="13"/>
-      <c r="O46" s="13"/>
-      <c r="P46" s="13"/>
-      <c r="Q46" s="13"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="15"/>
-    </row>
-    <row r="47" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
-      <c r="J47" s="13"/>
-      <c r="K47" s="13"/>
-      <c r="L47" s="13"/>
-      <c r="M47" s="13"/>
-      <c r="N47" s="13"/>
-      <c r="O47" s="13"/>
-      <c r="P47" s="13"/>
-      <c r="Q47" s="13"/>
-      <c r="R47" s="14"/>
-      <c r="S47" s="2"/>
-      <c r="T47" s="15"/>
-    </row>
-    <row r="48" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="13"/>
-      <c r="K48" s="13"/>
-      <c r="L48" s="13"/>
-      <c r="M48" s="13"/>
-      <c r="N48" s="13"/>
-      <c r="O48" s="13"/>
-      <c r="P48" s="13"/>
-      <c r="Q48" s="13"/>
-      <c r="R48" s="14"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="15"/>
-    </row>
-    <row r="49" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="13"/>
-      <c r="K49" s="13"/>
-      <c r="L49" s="13"/>
-      <c r="M49" s="13"/>
-      <c r="N49" s="13"/>
-      <c r="O49" s="13"/>
-      <c r="P49" s="13"/>
-      <c r="Q49" s="13"/>
-      <c r="R49" s="14"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="15"/>
-    </row>
-    <row r="50" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="13"/>
-      <c r="N50" s="13"/>
-      <c r="O50" s="13"/>
-      <c r="P50" s="13"/>
-      <c r="Q50" s="13"/>
-      <c r="R50" s="14"/>
-      <c r="S50" s="2"/>
-      <c r="T50" s="15"/>
-    </row>
-    <row r="51" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="13"/>
-      <c r="K51" s="13"/>
-      <c r="L51" s="13"/>
-      <c r="M51" s="13"/>
-      <c r="N51" s="13"/>
-      <c r="O51" s="13"/>
-      <c r="P51" s="13"/>
-      <c r="Q51" s="13"/>
-      <c r="R51" s="14"/>
-      <c r="S51" s="2"/>
-      <c r="T51" s="15"/>
-    </row>
-    <row r="52" spans="6:20" ht="14.25" customHeight="1">
+    <row r="32" spans="1:20" s="46" customFormat="1" ht="135.75" thickBot="1">
+      <c r="A32" s="20">
+        <v>16</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="F32" s="23">
+        <v>45057</v>
+      </c>
+      <c r="G32" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="H32" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="I32" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="J32" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="25"/>
+      <c r="O32" s="25"/>
+      <c r="P32" s="25"/>
+      <c r="Q32" s="25"/>
+      <c r="R32" s="26"/>
+      <c r="S32" s="27"/>
+      <c r="T32" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" s="46" customFormat="1" ht="135.75" thickBot="1">
+      <c r="A33" s="20">
+        <v>17</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="F33" s="23">
+        <v>45058</v>
+      </c>
+      <c r="G33" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="H33" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="I33" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="J33" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K33" s="25"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="25"/>
+      <c r="O33" s="25"/>
+      <c r="P33" s="25"/>
+      <c r="Q33" s="25"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="27"/>
+      <c r="T33" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" s="46" customFormat="1" ht="135.75" thickBot="1">
+      <c r="A34" s="20">
+        <v>18</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="F34" s="23">
+        <v>45058</v>
+      </c>
+      <c r="G34" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="H34" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="I34" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="J34" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="25"/>
+      <c r="Q34" s="25"/>
+      <c r="R34" s="26"/>
+      <c r="S34" s="27"/>
+      <c r="T34" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" s="46" customFormat="1" ht="135.75" thickBot="1">
+      <c r="A35" s="20">
+        <v>19</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F35" s="23">
+        <v>45058</v>
+      </c>
+      <c r="G35" s="32" t="s">
+        <v>228</v>
+      </c>
+      <c r="H35" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="I35" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="J35" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K35" s="25"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="25"/>
+      <c r="P35" s="25"/>
+      <c r="Q35" s="25"/>
+      <c r="R35" s="26"/>
+      <c r="S35" s="27"/>
+      <c r="T35" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" s="46" customFormat="1" ht="150.75" thickBot="1">
+      <c r="A36" s="20">
+        <v>33</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36" s="23">
+        <v>45058</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="H36" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="I36" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J36" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K36" s="25"/>
+      <c r="L36" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M36" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="N36" s="25"/>
+      <c r="O36" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="P36" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q36" s="25"/>
+      <c r="R36" s="26"/>
+      <c r="S36" s="27"/>
+      <c r="T36" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" s="46" customFormat="1" ht="165.75" thickBot="1">
+      <c r="A37" s="20">
+        <v>41</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" s="23">
+        <v>45058</v>
+      </c>
+      <c r="G37" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="H37" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="I37" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J37" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K37" s="25"/>
+      <c r="L37" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M37" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="N37" s="25"/>
+      <c r="O37" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="P37" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q37" s="25"/>
+      <c r="R37" s="26"/>
+      <c r="S37" s="27"/>
+      <c r="T37" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" s="46" customFormat="1" ht="45.75" thickBot="1">
+      <c r="A38" s="20">
+        <v>49</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F38" s="23"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="K38" s="25"/>
+      <c r="L38" s="25"/>
+      <c r="M38" s="25"/>
+      <c r="N38" s="25"/>
+      <c r="O38" s="25"/>
+      <c r="P38" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q38" s="25"/>
+      <c r="R38" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="S38" s="27"/>
+      <c r="T38" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" s="46" customFormat="1" ht="135.75" thickBot="1">
+      <c r="A39" s="20">
+        <v>94</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="F39" s="23">
+        <v>45057</v>
+      </c>
+      <c r="G39" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="H39" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="I39" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="J39" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M39" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="N39" s="25"/>
+      <c r="O39" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="P39" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q39" s="25"/>
+      <c r="R39" s="26"/>
+      <c r="S39" s="27"/>
+      <c r="T39" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" s="68" customFormat="1" ht="135.75" thickBot="1">
+      <c r="A40" s="59">
+        <v>95</v>
+      </c>
+      <c r="B40" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="60" t="s">
+        <v>172</v>
+      </c>
+      <c r="E40" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="F40" s="62"/>
+      <c r="G40" s="63"/>
+      <c r="H40" s="63"/>
+      <c r="I40" s="63"/>
+      <c r="J40" s="64" t="s">
+        <v>103</v>
+      </c>
+      <c r="K40" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="L40" s="64"/>
+      <c r="M40" s="64"/>
+      <c r="N40" s="64"/>
+      <c r="O40" s="64"/>
+      <c r="P40" s="64"/>
+      <c r="Q40" s="64"/>
+      <c r="R40" s="65"/>
+      <c r="S40" s="66"/>
+      <c r="T40" s="67" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" s="46" customFormat="1" ht="105.75" thickBot="1">
+      <c r="A41" s="20">
+        <v>96</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="F41" s="23">
+        <v>45057</v>
+      </c>
+      <c r="G41" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="H41" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="I41" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="J41" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K41" s="25"/>
+      <c r="L41" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M41" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="N41" s="25"/>
+      <c r="O41" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="P41" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q41" s="25"/>
+      <c r="R41" s="26"/>
+      <c r="S41" s="27"/>
+      <c r="T41" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" s="46" customFormat="1" ht="120.75" thickBot="1">
+      <c r="A42" s="20">
+        <v>97</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="F42" s="23">
+        <v>45057</v>
+      </c>
+      <c r="G42" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="H42" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="I42" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="J42" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M42" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="N42" s="25"/>
+      <c r="O42" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="P42" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q42" s="25"/>
+      <c r="R42" s="26"/>
+      <c r="S42" s="27"/>
+      <c r="T42" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" s="46" customFormat="1" ht="135.75" thickBot="1">
+      <c r="A43" s="20">
+        <v>98</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="F43" s="23">
+        <v>45057</v>
+      </c>
+      <c r="G43" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="H43" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="I43" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="J43" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K43" s="25"/>
+      <c r="L43" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M43" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="N43" s="25"/>
+      <c r="O43" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="P43" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q43" s="25"/>
+      <c r="R43" s="26"/>
+      <c r="S43" s="27"/>
+      <c r="T43" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" s="46" customFormat="1" ht="135.75" thickBot="1">
+      <c r="A44" s="20">
+        <v>99</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="F44" s="23">
+        <v>45057</v>
+      </c>
+      <c r="G44" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="H44" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="I44" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="J44" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K44" s="25"/>
+      <c r="L44" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M44" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="N44" s="25"/>
+      <c r="O44" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="P44" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q44" s="25"/>
+      <c r="R44" s="26"/>
+      <c r="S44" s="27"/>
+      <c r="T44" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" s="46" customFormat="1" ht="105.75" thickBot="1">
+      <c r="A45" s="20">
+        <v>100</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="F45" s="23">
+        <v>45057</v>
+      </c>
+      <c r="G45" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="H45" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="I45" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="J45" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K45" s="25"/>
+      <c r="L45" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M45" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="N45" s="25"/>
+      <c r="O45" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="P45" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q45" s="25"/>
+      <c r="R45" s="26"/>
+      <c r="S45" s="27"/>
+      <c r="T45" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" s="46" customFormat="1" ht="120.75" thickBot="1">
+      <c r="A46" s="20">
+        <v>101</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="F46" s="23">
+        <v>45057</v>
+      </c>
+      <c r="G46" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="H46" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="I46" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="J46" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K46" s="25"/>
+      <c r="L46" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M46" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="N46" s="25"/>
+      <c r="O46" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="P46" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q46" s="25"/>
+      <c r="R46" s="26"/>
+      <c r="S46" s="27"/>
+      <c r="T46" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" s="46" customFormat="1" ht="135.75" thickBot="1">
+      <c r="A47" s="20">
+        <v>102</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="F47" s="23">
+        <v>45057</v>
+      </c>
+      <c r="G47" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="H47" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="I47" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="J47" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="K47" s="25"/>
+      <c r="L47" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M47" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="N47" s="25"/>
+      <c r="O47" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="P47" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q47" s="25"/>
+      <c r="R47" s="26"/>
+      <c r="S47" s="27"/>
+      <c r="T47" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" s="46" customFormat="1" ht="135.75" thickBot="1">
+      <c r="A48" s="20">
+        <v>103</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="F48" s="23">
+        <v>45057</v>
+      </c>
+      <c r="G48" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="H48" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="I48" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="J48" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="K48" s="25"/>
+      <c r="L48" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M48" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="N48" s="25"/>
+      <c r="O48" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="P48" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q48" s="25"/>
+      <c r="R48" s="26"/>
+      <c r="S48" s="27"/>
+      <c r="T48" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" s="46" customFormat="1" ht="105.75" thickBot="1">
+      <c r="A49" s="20">
+        <v>104</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="F49" s="23">
+        <v>45057</v>
+      </c>
+      <c r="G49" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="H49" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="I49" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="J49" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="K49" s="25"/>
+      <c r="L49" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M49" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="N49" s="25"/>
+      <c r="O49" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="P49" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q49" s="25"/>
+      <c r="R49" s="26"/>
+      <c r="S49" s="27"/>
+      <c r="T49" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" s="46" customFormat="1" ht="135.75" thickBot="1">
+      <c r="A50" s="20">
+        <v>105</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="F50" s="23">
+        <v>45057</v>
+      </c>
+      <c r="G50" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="H50" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="I50" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="J50" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K50" s="25"/>
+      <c r="L50" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M50" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="N50" s="25"/>
+      <c r="O50" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="P50" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q50" s="25"/>
+      <c r="R50" s="26"/>
+      <c r="S50" s="27"/>
+      <c r="T50" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" s="68" customFormat="1" ht="135">
+      <c r="A51" s="59">
+        <v>106</v>
+      </c>
+      <c r="B51" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" s="60" t="s">
+        <v>214</v>
+      </c>
+      <c r="E51" s="61" t="s">
+        <v>215</v>
+      </c>
+      <c r="F51" s="23">
+        <v>45058</v>
+      </c>
+      <c r="G51" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="H51" s="69" t="s">
+        <v>231</v>
+      </c>
+      <c r="I51" s="63" t="s">
+        <v>232</v>
+      </c>
+      <c r="J51" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K51" s="63"/>
+      <c r="L51" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M51" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="N51" s="25"/>
+      <c r="O51" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="P51" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q51" s="64"/>
+      <c r="R51" s="65"/>
+      <c r="S51" s="66"/>
+      <c r="T51" s="67" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" ht="14.25" customHeight="1">
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
       <c r="H52" s="12"/>
@@ -5319,7 +6320,7 @@
       <c r="S52" s="2"/>
       <c r="T52" s="15"/>
     </row>
-    <row r="53" spans="6:20" ht="14.25" customHeight="1">
+    <row r="53" spans="1:20" ht="14.25" customHeight="1">
       <c r="F53" s="12"/>
       <c r="G53" s="12"/>
       <c r="H53" s="12"/>
@@ -5336,7 +6337,7 @@
       <c r="S53" s="2"/>
       <c r="T53" s="15"/>
     </row>
-    <row r="54" spans="6:20" ht="14.25" customHeight="1">
+    <row r="54" spans="1:20" ht="14.25" customHeight="1">
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
       <c r="H54" s="12"/>
@@ -5353,7 +6354,7 @@
       <c r="S54" s="2"/>
       <c r="T54" s="15"/>
     </row>
-    <row r="55" spans="6:20" ht="14.25" customHeight="1">
+    <row r="55" spans="1:20" ht="14.25" customHeight="1">
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
       <c r="H55" s="12"/>
@@ -5370,7 +6371,7 @@
       <c r="S55" s="2"/>
       <c r="T55" s="15"/>
     </row>
-    <row r="56" spans="6:20" ht="14.25" customHeight="1">
+    <row r="56" spans="1:20" ht="14.25" customHeight="1">
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
@@ -5387,7 +6388,7 @@
       <c r="S56" s="2"/>
       <c r="T56" s="15"/>
     </row>
-    <row r="57" spans="6:20" ht="14.25" customHeight="1">
+    <row r="57" spans="1:20" ht="14.25" customHeight="1">
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
@@ -5404,7 +6405,7 @@
       <c r="S57" s="2"/>
       <c r="T57" s="15"/>
     </row>
-    <row r="58" spans="6:20" ht="14.25" customHeight="1">
+    <row r="58" spans="1:20" ht="14.25" customHeight="1">
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
       <c r="H58" s="12"/>
@@ -5421,7 +6422,7 @@
       <c r="S58" s="2"/>
       <c r="T58" s="15"/>
     </row>
-    <row r="59" spans="6:20" ht="14.25" customHeight="1">
+    <row r="59" spans="1:20" ht="14.25" customHeight="1">
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
       <c r="H59" s="12"/>
@@ -5438,7 +6439,7 @@
       <c r="S59" s="2"/>
       <c r="T59" s="15"/>
     </row>
-    <row r="60" spans="6:20" ht="14.25" customHeight="1">
+    <row r="60" spans="1:20" ht="14.25" customHeight="1">
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
@@ -5455,7 +6456,7 @@
       <c r="S60" s="2"/>
       <c r="T60" s="15"/>
     </row>
-    <row r="61" spans="6:20" ht="14.25" customHeight="1">
+    <row r="61" spans="1:20" ht="14.25" customHeight="1">
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
       <c r="H61" s="12"/>
@@ -5472,7 +6473,7 @@
       <c r="S61" s="2"/>
       <c r="T61" s="15"/>
     </row>
-    <row r="62" spans="6:20" ht="14.25" customHeight="1">
+    <row r="62" spans="1:20" ht="14.25" customHeight="1">
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
       <c r="H62" s="12"/>
@@ -5489,7 +6490,7 @@
       <c r="S62" s="2"/>
       <c r="T62" s="15"/>
     </row>
-    <row r="63" spans="6:20" ht="14.25" customHeight="1">
+    <row r="63" spans="1:20" ht="14.25" customHeight="1">
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
       <c r="H63" s="12"/>
@@ -5506,7 +6507,7 @@
       <c r="S63" s="2"/>
       <c r="T63" s="15"/>
     </row>
-    <row r="64" spans="6:20" ht="14.25" customHeight="1">
+    <row r="64" spans="1:20" ht="14.25" customHeight="1">
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
       <c r="H64" s="12"/>
@@ -14559,7 +15560,7 @@
       <c r="T649" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T31" xr:uid="{00000000-0009-0000-0000-000002000000}">
+  <autoFilter ref="A9:T51" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:T31">
       <sortCondition ref="B9:B31"/>
     </sortState>
@@ -14583,7 +15584,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J22:J31 O10:O31 L10:M31 J10:J20</xm:sqref>
+          <xm:sqref>J22:J31 O10:O31 J10:J20 L10:M31</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
@@ -16660,6 +17661,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A4E8F9A681C30D41B0A35D53CC971FDB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03b261b6ced3636c743b9d34d46eef88">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65eedeea-c684-4a28-bcc9-4d463688c730" xmlns:ns3="776b4d22-7036-4a85-b669-c340da9bc363" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c72f12b0b17737fbc805bf10a31e1c9f" ns2:_="" ns3:_="">
     <xsd:import namespace="65eedeea-c684-4a28-bcc9-4d463688c730"/>
@@ -16824,16 +17834,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{767D3CD0-FCF6-49F3-A5DC-793CA28F171B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6456830E-E76B-4F9B-B4C4-75534FEFA7DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16850,12 +17859,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{767D3CD0-FCF6-49F3-A5DC-793CA28F171B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Submit accreditamento scheda vaccinazione e Certificato Vaccinale - update files
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DXCTECHNOLO/dxc/sinfonia-vaccini/2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111DXCTECHNOLO/dxc/sinfonia-vaccini/2.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asaginario\Documents\Lavoro\Progetti\SGISanita-Projects\FSE-TestCaseAccreditamento\GATEWAY\A1#111DXCTECHNOLO\dxc\sinfonia-vaccini\2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB5D104-DA9D-426C-89AC-F3041DDE2D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC4A823-6360-4521-8F2F-E305EAB1E4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -691,33 +691,6 @@
 </t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.204.859f21dd3c5c72a507efab6bd3cdb8c396219efeddd908bae22a9dc478620663.f893506039^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>e73ca0da12f05010</t>
-  </si>
-  <si>
-    <t>044e5a72af030b16</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.204.5bf77ae1f2bf7ff257aeaabd5b70411325a89b3a6ff52d5ed0b5663cca6941f5.5f50ee1b06^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>d7b1d8ac3efc2ee2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.204.859f21dd3c5c72a507efab6bd3cdb8c396219efeddd908bae22a9dc478620663.f50ddf5906^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-10T14:29:20Z</t>
-  </si>
-  <si>
-    <t>2023-05-10T14:23:20Z</t>
-  </si>
-  <si>
-    <t>2023-05-10T14:14:30Z</t>
-  </si>
-  <si>
     <t>2023-05-10T14:14:19Z</t>
   </si>
   <si>
@@ -947,33 +920,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-05-10T15:29:20Z</t>
-  </si>
-  <si>
-    <t>0fb5479234f1c0bf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.904.75877f466c4515833b756f7f42b551491927b78b2775850632f26c9ce055839e.84c1e16cee^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-12T10:41:20Z</t>
-  </si>
-  <si>
-    <t>65354110eee60ae0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.904.0caa65f702128f218163d49362d1e8faafd3ee1502e7cfbf3c5ff04731a06f50.9c69c3c3a1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-12T11:41:20Z</t>
-  </si>
-  <si>
-    <t>366754ad0c6013b5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.904.8c21ca1b2e018ded516266256778abe98e9e25498ac781019ad87b7f3b325132.dcfd4184cb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-05-12T15:29:20Z</t>
   </si>
   <si>
@@ -986,16 +932,70 @@
     <t>2023-05-12T13:41:20Z</t>
   </si>
   <si>
-    <t>118eca65cdd9a86a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.904.50b3dc5d32cc3e16e4330e4a4d36eeabcdea780d84aaed797129d80d5785674c.df1e9621b7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>418d4d71fd12ba03</t>
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150.4.4.904.8c21ca1b2e018ded516266256778abe98e9e25498ac781019ad87b7f3b325132.31a3a04055^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-24T14:14:30Z</t>
+  </si>
+  <si>
+    <t>c114460dc8128a73</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.204.859f21dd3c5c72a507efab6bd3cdb8c396219efeddd908bae22a9dc478620663.d8ca236c93^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-24T14:23:20Z</t>
+  </si>
+  <si>
+    <t>befeddd00242b3a7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.204.5bf77ae1f2bf7ff257aeaabd5b70411325a89b3a6ff52d5ed0b5663cca6941f5.0e6d7d15db^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.204.859f21dd3c5c72a507efab6bd3cdb8c396219efeddd908bae22a9dc478620663.6cbc8fabe6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>89e89fa32743878e</t>
+  </si>
+  <si>
+    <t>2023-05-24T24:29:20Z</t>
+  </si>
+  <si>
+    <t>2023-05-24T15:29:20Z</t>
+  </si>
+  <si>
+    <t>0e2caeea83a5ed94</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.75877f466c4515833b756f7f42b551491927b78b2775850632f26c9ce055839e.fa53a62201^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>d07a9b936df2fb51</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.0caa65f702128f218163d49362d1e8faafd3ee1502e7cfbf3c5ff04731a06f50.1944f08f76^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2a0fe8dd683d03fd</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.8c21ca1b2e018ded516266256778abe98e9e25498ac781019ad87b7f3b325132.dac25e0680^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>7f04747accdebf5b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.904.50b3dc5d32cc3e16e4330e4a4d36eeabcdea780d84aaed797129d80d5785674c.2b9daf5b67^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-24T11:41:20Z</t>
+  </si>
+  <si>
+    <t>2023-05-24T10:41:20Zs</t>
   </si>
 </sst>
 </file>
@@ -1467,28 +1467,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1522,6 +1500,28 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3977,13 +3977,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:T649"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="F46" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="L55" sqref="L55"/>
+      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4022,12 +4023,12 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="62"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -4045,14 +4046,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="58" t="s">
+      <c r="B3" s="65"/>
+      <c r="C3" s="70" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="50"/>
+      <c r="D3" s="62"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -4070,12 +4071,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="58" t="s">
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="D4" s="50"/>
+      <c r="D4" s="62"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -4094,12 +4095,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="56"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="58" t="s">
+      <c r="A5" s="68"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="50"/>
+      <c r="D5" s="62"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4117,8 +4118,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="47"/>
-      <c r="B6" s="48"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4235,7 +4236,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="150.75" thickBot="1">
+    <row r="10" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A10" s="20">
         <v>20</v>
       </c>
@@ -4255,7 +4256,7 @@
         <v>45056</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="H10" s="32" t="s">
         <v>140</v>
@@ -4279,7 +4280,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="150.75" thickBot="1">
+    <row r="11" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A11" s="20">
         <v>21</v>
       </c>
@@ -4296,16 +4297,16 @@
         <v>52</v>
       </c>
       <c r="F11" s="23">
-        <v>45056</v>
+        <v>45070</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>149</v>
+        <v>213</v>
       </c>
       <c r="H11" s="32" t="s">
-        <v>142</v>
+        <v>214</v>
       </c>
       <c r="I11" s="32" t="s">
-        <v>141</v>
+        <v>215</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>62</v>
@@ -4323,7 +4324,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="150.75" thickBot="1">
+    <row r="12" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A12" s="20">
         <v>22</v>
       </c>
@@ -4340,16 +4341,16 @@
         <v>54</v>
       </c>
       <c r="F12" s="23">
-        <v>45056</v>
+        <v>45070</v>
       </c>
       <c r="G12" s="32" t="s">
-        <v>148</v>
+        <v>216</v>
       </c>
       <c r="H12" s="32" t="s">
-        <v>143</v>
+        <v>217</v>
       </c>
       <c r="I12" s="32" t="s">
-        <v>144</v>
+        <v>218</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>62</v>
@@ -4367,7 +4368,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="150.75" thickBot="1">
+    <row r="13" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A13" s="20">
         <v>23</v>
       </c>
@@ -4384,16 +4385,16 @@
         <v>56</v>
       </c>
       <c r="F13" s="23">
-        <v>45056</v>
+        <v>45070</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>147</v>
+        <v>221</v>
       </c>
       <c r="H13" s="32" t="s">
-        <v>145</v>
+        <v>220</v>
       </c>
       <c r="I13" s="32" t="s">
-        <v>146</v>
+        <v>219</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>62</v>
@@ -4411,7 +4412,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="150.75" thickBot="1">
+    <row r="14" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A14" s="20">
         <v>34</v>
       </c>
@@ -4463,7 +4464,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="165.75" thickBot="1">
+    <row r="15" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A15" s="20">
         <v>42</v>
       </c>
@@ -4515,7 +4516,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="45.75" thickBot="1">
+    <row r="16" spans="1:20" ht="45.75" hidden="1" thickBot="1">
       <c r="A16" s="20">
         <v>50</v>
       </c>
@@ -4544,7 +4545,7 @@
       <c r="N16" s="25"/>
       <c r="O16" s="25"/>
       <c r="P16" s="33" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="26" t="s">
@@ -4555,7 +4556,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="120.75" thickBot="1">
+    <row r="17" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A17" s="20">
         <v>107</v>
       </c>
@@ -4595,7 +4596,7 @@
       </c>
       <c r="N17" s="25"/>
       <c r="O17" s="25" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="P17" s="25" t="s">
         <v>106</v>
@@ -4607,7 +4608,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="45" customFormat="1" ht="120.75" thickBot="1">
+    <row r="18" spans="1:20" s="45" customFormat="1" ht="120.75" hidden="1" thickBot="1">
       <c r="A18" s="36">
         <v>108</v>
       </c>
@@ -4645,7 +4646,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="120.75" thickBot="1">
+    <row r="19" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A19" s="20">
         <v>109</v>
       </c>
@@ -4665,13 +4666,13 @@
         <v>45057</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="H19" s="34" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I19" s="32" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>62</v>
@@ -4685,7 +4686,7 @@
       </c>
       <c r="N19" s="25"/>
       <c r="O19" s="25" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="P19" s="25" t="s">
         <v>106</v>
@@ -4697,7 +4698,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="105.75" thickBot="1">
+    <row r="20" spans="1:20" ht="105.75" hidden="1" thickBot="1">
       <c r="A20" s="20">
         <v>110</v>
       </c>
@@ -4749,7 +4750,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="120.75" thickBot="1">
+    <row r="21" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A21" s="20">
         <v>111</v>
       </c>
@@ -4789,7 +4790,7 @@
       </c>
       <c r="N21" s="25"/>
       <c r="O21" s="25" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="P21" s="25" t="s">
         <v>106</v>
@@ -4801,7 +4802,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="120.75" thickBot="1">
+    <row r="22" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A22" s="20">
         <v>112</v>
       </c>
@@ -4830,7 +4831,7 @@
         <v>116</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="K22" s="25"/>
       <c r="L22" s="25" t="s">
@@ -4841,7 +4842,7 @@
       </c>
       <c r="N22" s="25"/>
       <c r="O22" s="25" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="P22" s="25" t="s">
         <v>106</v>
@@ -4853,7 +4854,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="120.75" thickBot="1">
+    <row r="23" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A23" s="20">
         <v>113</v>
       </c>
@@ -4882,7 +4883,7 @@
         <v>118</v>
       </c>
       <c r="J23" s="25" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="K23" s="25"/>
       <c r="L23" s="25" t="s">
@@ -4905,7 +4906,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="120.75" thickBot="1">
+    <row r="24" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A24" s="20">
         <v>114</v>
       </c>
@@ -4957,7 +4958,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="120.75" thickBot="1">
+    <row r="25" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A25" s="20">
         <v>115</v>
       </c>
@@ -5009,7 +5010,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="120.75" thickBot="1">
+    <row r="26" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A26" s="20">
         <v>116</v>
       </c>
@@ -5061,7 +5062,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="120.75" thickBot="1">
+    <row r="27" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A27" s="20">
         <v>117</v>
       </c>
@@ -5113,7 +5114,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="120.75" thickBot="1">
+    <row r="28" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A28" s="20">
         <v>118</v>
       </c>
@@ -5165,7 +5166,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="120.75" thickBot="1">
+    <row r="29" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A29" s="20">
         <v>119</v>
       </c>
@@ -5217,7 +5218,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="120.75" thickBot="1">
+    <row r="30" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A30" s="20">
         <v>120</v>
       </c>
@@ -5269,7 +5270,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="120.75" thickBot="1">
+    <row r="31" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A31" s="20">
         <v>121</v>
       </c>
@@ -5332,22 +5333,22 @@
         <v>46</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F32" s="23">
-        <v>45057</v>
+        <v>45070</v>
       </c>
       <c r="G32" s="32" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H32" s="32" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="I32" s="32" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="J32" s="25" t="s">
         <v>62</v>
@@ -5376,22 +5377,22 @@
         <v>46</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F33" s="23">
-        <v>45058</v>
+        <v>45070</v>
       </c>
       <c r="G33" s="32" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="H33" s="32" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="I33" s="32" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="J33" s="25" t="s">
         <v>62</v>
@@ -5420,22 +5421,22 @@
         <v>46</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="F34" s="23">
-        <v>45058</v>
+        <v>45070</v>
       </c>
       <c r="G34" s="32" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="H34" s="32" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="I34" s="32" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="J34" s="25" t="s">
         <v>62</v>
@@ -5464,16 +5465,16 @@
         <v>46</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="F35" s="23">
-        <v>45058</v>
+        <v>45070</v>
       </c>
       <c r="G35" s="32" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="H35" s="32" t="s">
         <v>229</v>
@@ -5508,7 +5509,7 @@
         <v>46</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E36" s="22" t="s">
         <v>57</v>
@@ -5517,10 +5518,10 @@
         <v>45058</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="H36" s="24" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="I36" s="24" t="s">
         <v>105</v>
@@ -5560,7 +5561,7 @@
         <v>46</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E37" s="22" t="s">
         <v>60</v>
@@ -5569,10 +5570,10 @@
         <v>45058</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="H37" s="24" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="I37" s="24" t="s">
         <v>105</v>
@@ -5612,7 +5613,7 @@
         <v>46</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E38" s="22" t="s">
         <v>61</v>
@@ -5630,7 +5631,7 @@
       <c r="N38" s="25"/>
       <c r="O38" s="25"/>
       <c r="P38" s="33" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="Q38" s="25"/>
       <c r="R38" s="26" t="s">
@@ -5652,22 +5653,22 @@
         <v>46</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="F39" s="23">
         <v>45057</v>
       </c>
       <c r="G39" s="32" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H39" s="24" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="I39" s="24" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="J39" s="25" t="s">
         <v>62</v>
@@ -5684,7 +5685,7 @@
         <v>62</v>
       </c>
       <c r="P39" s="33" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="Q39" s="25"/>
       <c r="R39" s="26"/>
@@ -5693,41 +5694,41 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:20" s="68" customFormat="1" ht="135.75" thickBot="1">
-      <c r="A40" s="59">
+    <row r="40" spans="1:20" s="56" customFormat="1" ht="135.75" thickBot="1">
+      <c r="A40" s="47">
         <v>95</v>
       </c>
-      <c r="B40" s="60" t="s">
+      <c r="B40" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="60" t="s">
+      <c r="C40" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="60" t="s">
-        <v>172</v>
-      </c>
-      <c r="E40" s="61" t="s">
-        <v>173</v>
-      </c>
-      <c r="F40" s="62"/>
-      <c r="G40" s="63"/>
-      <c r="H40" s="63"/>
-      <c r="I40" s="63"/>
-      <c r="J40" s="64" t="s">
+      <c r="D40" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="E40" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="F40" s="50"/>
+      <c r="G40" s="51"/>
+      <c r="H40" s="51"/>
+      <c r="I40" s="51"/>
+      <c r="J40" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="K40" s="64" t="s">
+      <c r="K40" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="L40" s="64"/>
-      <c r="M40" s="64"/>
-      <c r="N40" s="64"/>
-      <c r="O40" s="64"/>
-      <c r="P40" s="64"/>
-      <c r="Q40" s="64"/>
-      <c r="R40" s="65"/>
-      <c r="S40" s="66"/>
-      <c r="T40" s="67" t="s">
+      <c r="L40" s="52"/>
+      <c r="M40" s="52"/>
+      <c r="N40" s="52"/>
+      <c r="O40" s="52"/>
+      <c r="P40" s="52"/>
+      <c r="Q40" s="52"/>
+      <c r="R40" s="53"/>
+      <c r="S40" s="54"/>
+      <c r="T40" s="55" t="s">
         <v>45</v>
       </c>
     </row>
@@ -5742,22 +5743,22 @@
         <v>46</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="F41" s="23">
         <v>45057</v>
       </c>
       <c r="G41" s="32" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H41" s="24" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="I41" s="24" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>62</v>
@@ -5794,22 +5795,22 @@
         <v>46</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="F42" s="23">
         <v>45057</v>
       </c>
       <c r="G42" s="32" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H42" s="24" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="I42" s="24" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="J42" s="33" t="s">
         <v>62</v>
@@ -5846,22 +5847,22 @@
         <v>46</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F43" s="23">
         <v>45057</v>
       </c>
       <c r="G43" s="32" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H43" s="24" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="J43" s="25" t="s">
         <v>62</v>
@@ -5898,22 +5899,22 @@
         <v>46</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F44" s="23">
         <v>45057</v>
       </c>
       <c r="G44" s="32" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H44" s="24" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="I44" s="24" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="J44" s="25" t="s">
         <v>62</v>
@@ -5950,22 +5951,22 @@
         <v>46</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="F45" s="23">
         <v>45057</v>
       </c>
       <c r="G45" s="32" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H45" s="24" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I45" s="24" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="J45" s="25" t="s">
         <v>62</v>
@@ -6002,22 +6003,22 @@
         <v>46</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F46" s="23">
         <v>45057</v>
       </c>
       <c r="G46" s="32" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H46" s="24" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="I46" s="24" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="J46" s="25" t="s">
         <v>62</v>
@@ -6054,22 +6055,22 @@
         <v>46</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F47" s="23">
         <v>45057</v>
       </c>
       <c r="G47" s="32" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J47" s="33" t="s">
         <v>62</v>
@@ -6106,22 +6107,22 @@
         <v>46</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F48" s="23">
         <v>45057</v>
       </c>
       <c r="G48" s="32" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H48" s="24" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="I48" s="24" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="J48" s="33" t="s">
         <v>62</v>
@@ -6158,22 +6159,22 @@
         <v>46</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="F49" s="23">
         <v>45057</v>
       </c>
       <c r="G49" s="32" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H49" s="24" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="I49" s="24" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="J49" s="33" t="s">
         <v>62</v>
@@ -6210,22 +6211,22 @@
         <v>46</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="F50" s="23">
         <v>45057</v>
       </c>
       <c r="G50" s="32" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H50" s="24" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="J50" s="25" t="s">
         <v>62</v>
@@ -6251,38 +6252,38 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:20" s="68" customFormat="1" ht="135">
-      <c r="A51" s="59">
+    <row r="51" spans="1:20" s="56" customFormat="1" ht="135">
+      <c r="A51" s="47">
         <v>106</v>
       </c>
-      <c r="B51" s="60" t="s">
+      <c r="B51" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="60" t="s">
+      <c r="C51" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="D51" s="60" t="s">
-        <v>214</v>
-      </c>
-      <c r="E51" s="61" t="s">
-        <v>215</v>
+      <c r="D51" s="48" t="s">
+        <v>205</v>
+      </c>
+      <c r="E51" s="49" t="s">
+        <v>206</v>
       </c>
       <c r="F51" s="23">
         <v>45058</v>
       </c>
-      <c r="G51" s="63" t="s">
-        <v>225</v>
-      </c>
-      <c r="H51" s="69" t="s">
-        <v>231</v>
-      </c>
-      <c r="I51" s="63" t="s">
-        <v>232</v>
-      </c>
-      <c r="J51" s="70" t="s">
+      <c r="G51" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="H51" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="I51" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="J51" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="K51" s="63"/>
+      <c r="K51" s="51"/>
       <c r="L51" s="25" t="s">
         <v>62</v>
       </c>
@@ -6296,10 +6297,10 @@
       <c r="P51" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="Q51" s="64"/>
-      <c r="R51" s="65"/>
-      <c r="S51" s="66"/>
-      <c r="T51" s="67" t="s">
+      <c r="Q51" s="52"/>
+      <c r="R51" s="53"/>
+      <c r="S51" s="54"/>
+      <c r="T51" s="55" t="s">
         <v>45</v>
       </c>
     </row>
@@ -15561,6 +15562,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:T51" xr:uid="{00000000-0009-0000-0000-000002000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="CERT_VAC"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:T31">
       <sortCondition ref="B9:B31"/>
     </sortState>
@@ -17661,15 +17667,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A4E8F9A681C30D41B0A35D53CC971FDB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03b261b6ced3636c743b9d34d46eef88">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65eedeea-c684-4a28-bcc9-4d463688c730" xmlns:ns3="776b4d22-7036-4a85-b669-c340da9bc363" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c72f12b0b17737fbc805bf10a31e1c9f" ns2:_="" ns3:_="">
     <xsd:import namespace="65eedeea-c684-4a28-bcc9-4d463688c730"/>
@@ -17834,15 +17831,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{767D3CD0-FCF6-49F3-A5DC-793CA28F171B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6456830E-E76B-4F9B-B4C4-75534FEFA7DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17859,4 +17857,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{767D3CD0-FCF6-49F3-A5DC-793CA28F171B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>